<commit_message>
ftp and map updates
</commit_message>
<xml_diff>
--- a/weather.xlsx
+++ b/weather.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TULPAR\2022\OzgunGorev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TULPAR\2022\tulpar-interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D3F6C8-6D36-4A31-B350-97127FCF98A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F086D9-9829-48B9-8F3B-D20B6BD37E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20B57456-6CA5-4450-BF1B-08F8CDB8E314}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{20B57456-6CA5-4450-BF1B-08F8CDB8E314}"/>
   </bookViews>
   <sheets>
     <sheet name="previous" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>Max_Temp</t>
   </si>
@@ -48,19 +48,158 @@
   </si>
   <si>
     <t>Rainfall</t>
+  </si>
+  <si>
+    <t>26.4</t>
+  </si>
+  <si>
+    <t>18.7</t>
+  </si>
+  <si>
+    <t>53.6</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>30.3</t>
+  </si>
+  <si>
+    <t>16.3</t>
+  </si>
+  <si>
+    <t>53.0</t>
+  </si>
+  <si>
+    <t>28.2</t>
+  </si>
+  <si>
+    <t>18.3</t>
+  </si>
+  <si>
+    <t>52.4</t>
+  </si>
+  <si>
+    <t>27.8</t>
+  </si>
+  <si>
+    <t>17.1</t>
+  </si>
+  <si>
+    <t>47.0</t>
+  </si>
+  <si>
+    <t>26.9</t>
+  </si>
+  <si>
+    <t>15.9</t>
+  </si>
+  <si>
+    <t>50.5</t>
+  </si>
+  <si>
+    <t>29.5</t>
+  </si>
+  <si>
+    <t>16.2</t>
+  </si>
+  <si>
+    <t>41.3</t>
+  </si>
+  <si>
+    <t>32.5</t>
+  </si>
+  <si>
+    <t>17.4</t>
+  </si>
+  <si>
+    <t>41.1</t>
+  </si>
+  <si>
+    <t>33.3</t>
+  </si>
+  <si>
+    <t>18.1</t>
+  </si>
+  <si>
+    <t>34.7</t>
+  </si>
+  <si>
+    <t>34.2</t>
+  </si>
+  <si>
+    <t>19.7</t>
+  </si>
+  <si>
+    <t>31.4</t>
+  </si>
+  <si>
+    <t>31.6</t>
+  </si>
+  <si>
+    <t>19.1</t>
+  </si>
+  <si>
+    <t>42.5</t>
+  </si>
+  <si>
+    <t>31.8</t>
+  </si>
+  <si>
+    <t>19.0</t>
+  </si>
+  <si>
+    <t>43.1</t>
+  </si>
+  <si>
+    <t>30.9</t>
+  </si>
+  <si>
+    <t>19.3</t>
+  </si>
+  <si>
+    <t>37.4</t>
+  </si>
+  <si>
+    <t>28.8</t>
+  </si>
+  <si>
+    <t>17.8</t>
+  </si>
+  <si>
+    <t>41.7</t>
+  </si>
+  <si>
+    <t>29.9</t>
+  </si>
+  <si>
+    <t>48.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="SansSerif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -81,14 +220,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{E29FAFAF-D010-4C46-85AD-05F64DF23233}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -402,11 +549,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9338673-8392-4F5A-B2F4-5BF306CAC518}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" customWidth="1"/>
@@ -414,7 +561,7 @@
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,200 +575,200 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B2">
-        <v>22</v>
-      </c>
-      <c r="C2">
-        <v>28</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>34</v>
-      </c>
-      <c r="B3">
-        <v>22</v>
-      </c>
-      <c r="C3">
-        <v>30</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>28</v>
-      </c>
-      <c r="B4">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>31</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>28</v>
-      </c>
-      <c r="B5">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>29</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>28</v>
-      </c>
-      <c r="B6">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>34</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>29</v>
-      </c>
-      <c r="B7">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>37</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>30</v>
-      </c>
-      <c r="B8">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>29</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>31</v>
-      </c>
-      <c r="B9">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>30</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>31</v>
-      </c>
-      <c r="B10">
-        <v>18</v>
-      </c>
-      <c r="C10">
-        <v>28</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>32</v>
-      </c>
-      <c r="B11">
-        <v>16</v>
-      </c>
-      <c r="C11">
-        <v>32</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>33</v>
-      </c>
-      <c r="B12">
-        <v>17</v>
-      </c>
-      <c r="C12">
-        <v>31</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>34</v>
-      </c>
-      <c r="B13">
-        <v>18</v>
-      </c>
-      <c r="C13">
-        <v>35</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>33</v>
-      </c>
-      <c r="B14">
-        <v>19</v>
-      </c>
-      <c r="C14">
-        <v>29</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>33</v>
-      </c>
-      <c r="B15">
-        <v>19</v>
-      </c>
-      <c r="C15">
-        <v>33</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -633,13 +780,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CBB38E-79B5-40B0-9686-B5F43937E09B}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -653,99 +800,99 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>18</v>
       </c>
       <c r="C3">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>18</v>
       </c>
       <c r="C4">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
         <v>34</v>
-      </c>
-      <c r="B6">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>30</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>33</v>
       </c>
       <c r="B8">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D8">
         <v>0</v>

</xml_diff>